<commit_message>
feat: Implement game session management and user integration
- Added functions to fetch game sessions by wallet address and current active session.
- Implemented user creation and session management in createGameSession function.
- Included user information in the returned game session object.
- Enhanced the fetchGameSessionsByAddress and fetchCurrentActiveSession functions to include user data.
- Updated the Prisma schema to ensure proper relationships between GameSession and User models.
- Refactored the useGame hook to accommodate new session management features.
- Improved error handling in KOL fetching functions.
</commit_message>
<xml_diff>
--- a/Radar Demo.xlsx
+++ b/Radar Demo.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plaum\Desktop\Soddle\Radar Hackathon\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F85B66-AF2E-4712-8269-F2A4FF319A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="25380" windowHeight="11320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Celebrities" sheetId="1" r:id="rId1"/>
     <sheet name="Riddle 1" sheetId="2" r:id="rId2"/>
     <sheet name="Descriptions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -164,6 +166,15 @@
     <t>https://x.com/IGGYAZALEA</t>
   </si>
   <si>
+    <t>vibhu</t>
+  </si>
+  <si>
+    <t>https://x.com/vibhu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country </t>
+  </si>
+  <si>
     <t>Age</t>
   </si>
   <si>
@@ -188,6 +199,9 @@
     <t>200-300k</t>
   </si>
   <si>
+    <t>Artificial</t>
+  </si>
+  <si>
     <t>NFTs</t>
   </si>
   <si>
@@ -212,9 +226,6 @@
     <t>England</t>
   </si>
   <si>
-    <t>Artificial</t>
-  </si>
-  <si>
     <t>41-50</t>
   </si>
   <si>
@@ -230,6 +241,9 @@
     <t>Founder</t>
   </si>
   <si>
+    <t>Canada</t>
+  </si>
+  <si>
     <t>NFTs, Founder</t>
   </si>
   <si>
@@ -245,9 +259,6 @@
     <t>Influencer</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>Influencer, NFTs</t>
   </si>
   <si>
@@ -260,6 +271,9 @@
     <t>Australia</t>
   </si>
   <si>
+    <t>India</t>
+  </si>
+  <si>
     <t>Description 1</t>
   </si>
   <si>
@@ -395,15 +409,6 @@
     <t>Trying to make crypto mainstream in her own way, you gotta respect it.</t>
   </si>
   <si>
-    <t>vibhu</t>
-  </si>
-  <si>
-    <t>https://x.com/vibhu</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>Has a lot of drip.</t>
   </si>
   <si>
@@ -411,21 +416,24 @@
   </si>
   <si>
     <t>Not into tokens or DeFi. NGMI except he already made it.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -433,25 +441,354 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -459,31 +796,313 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -532,7 +1151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -567,7 +1186,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -741,31 +1360,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C25" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="16.8" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.3671875" customWidth="1"/>
+    <col min="3" max="3" width="28.546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -787,7 +1401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -798,7 +1412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -809,7 +1423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -820,7 +1434,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -831,7 +1445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -842,7 +1456,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -853,7 +1467,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -864,7 +1478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -875,7 +1489,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -886,7 +1500,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -897,7 +1511,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -908,7 +1522,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -919,7 +1533,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -930,49 +1544,51 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{5F7990B8-DED6-4C02-8FAB-5F9BDE111825}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{C0C2F6D3-5CCA-49EC-ADB1-38D0BBC58B95}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{2A6E46A8-F46B-485A-9640-C16B10C5CCDF}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{7CF9CC9F-C4BB-40BE-B89C-DAF38A44E1F9}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://x.com/frankdegods"/>
+    <hyperlink ref="C10" r:id="rId2" display="https://x.com/armaniferrante"/>
+    <hyperlink ref="C6" r:id="rId3" display="https://x.com/kashdhanda"/>
+    <hyperlink ref="C4" r:id="rId4" display="https://x.com/calilyliu"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B593AD-C89F-4678-A3E6-EC15C645E210}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J9" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.3671875" customWidth="1"/>
+    <col min="3" max="3" width="27.3671875" customWidth="1"/>
+    <col min="4" max="4" width="17.2734375" customWidth="1"/>
+    <col min="6" max="6" width="21.546875" customWidth="1"/>
+    <col min="7" max="7" width="15.09375" customWidth="1"/>
+    <col min="8" max="8" width="13.2734375" customWidth="1"/>
+    <col min="9" max="9" width="14.8203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -983,25 +1599,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1012,25 +1628,25 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <v>2021</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1041,25 +1657,25 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F4">
         <v>2009</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1070,25 +1686,25 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F5">
         <v>2009</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1099,25 +1715,25 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F6">
         <v>2013</v>
       </c>
       <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
         <v>56</v>
       </c>
-      <c r="H6" t="s">
-        <v>61</v>
-      </c>
       <c r="I6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1128,25 +1744,25 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F7">
         <v>2011</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1157,25 +1773,25 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F8">
         <v>2008</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1186,25 +1802,25 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F9">
         <v>2020</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1215,25 +1831,25 @@
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F10">
         <v>2011</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1244,25 +1860,25 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F11">
         <v>2010</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1273,25 +1889,25 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F12">
         <v>2014</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1302,25 +1918,25 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F13">
         <v>2012</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1331,25 +1947,25 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F14">
         <v>2022</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1360,25 +1976,25 @@
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F15">
         <v>2021</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1388,84 +2004,86 @@
       <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>76</v>
+      <c r="D16" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F16" s="1">
         <v>2010</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F17">
         <v>2008</v>
       </c>
       <c r="G17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
         <v>56</v>
       </c>
-      <c r="H17" t="s">
-        <v>61</v>
-      </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{F27A5AE1-2CE5-44D5-B16D-70E5A7A54AD4}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{BA119A74-1A4F-4A93-A0D3-05E2264C0B49}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{08C7C56C-28D9-4BD9-81C3-13E6401D9344}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{4DB2D4D7-AD15-43D2-A2E2-8B2D92E765AD}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://x.com/frankdegods"/>
+    <hyperlink ref="C10" r:id="rId2" display="https://x.com/armaniferrante"/>
+    <hyperlink ref="C6" r:id="rId3" display="https://x.com/kashdhanda"/>
+    <hyperlink ref="C4" r:id="rId4" display="https://x.com/calilyliu"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE3F87D-98FF-47C7-B4C2-38E8B9AF0585}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D20" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.8" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="15.90625" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.09375" customWidth="1"/>
     <col min="3" max="3" width="26.7265625" customWidth="1"/>
     <col min="4" max="4" width="67.1796875" customWidth="1"/>
     <col min="5" max="5" width="86" customWidth="1"/>
-    <col min="6" max="6" width="62.08984375" customWidth="1"/>
+    <col min="6" max="6" width="62.09375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1476,16 +2094,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1496,16 +2114,16 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1516,16 +2134,16 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1536,16 +2154,16 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1556,16 +2174,16 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1576,16 +2194,16 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1596,16 +2214,16 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1616,16 +2234,16 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1636,16 +2254,16 @@
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1656,16 +2274,16 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1676,16 +2294,16 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1696,16 +2314,16 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1716,16 +2334,16 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1736,16 +2354,16 @@
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1756,42 +2374,43 @@
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{047B0ADB-B8F3-4EBB-AAEE-24ACD63FB893}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{CFE5A3CD-8A84-471D-806B-A9FE5418C2D7}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{7EE6CBD3-64DA-483F-988D-FBA22AC3365F}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{23636F5E-150F-4AF4-889C-4F46C5DD8F3C}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://x.com/frankdegods"/>
+    <hyperlink ref="C10" r:id="rId2" display="https://x.com/armaniferrante"/>
+    <hyperlink ref="C6" r:id="rId3" display="https://x.com/kashdhanda"/>
+    <hyperlink ref="C4" r:id="rId4" display="https://x.com/calilyliu"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>